<commit_message>
added high temp industrial heat
</commit_message>
<xml_diff>
--- a/sector_breakdown/Industry/nonmetallic_industries_energy_cons.xlsx
+++ b/sector_breakdown/Industry/nonmetallic_industries_energy_cons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU_Man/h2_system_dynamics/sector_breakdown/Industry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76FECF56-9D06-48A4-99FA-702ECEA1174A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{76FECF56-9D06-48A4-99FA-702ECEA1174A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0D2ACBA-5A69-4E6E-998D-52D0D9F7D62B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -474,12 +474,14 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -487,8 +489,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,22 +903,22 @@
       <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1207,40 +1207,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>51940.143999999993</v>
       </c>
@@ -3140,40 +3140,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4534,11 +4534,11 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>266085.32900000003</v>
       </c>
-      <c r="M45" s="24">
+      <c r="M45" s="21">
         <f>'Sheet 2'!L45+'Sheet 3'!L45+'Sheet 4'!L45</f>
         <v>184883.56300000002</v>
       </c>
@@ -4664,40 +4664,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -6058,7 +6058,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>34100.144</v>
       </c>
@@ -6184,40 +6184,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7578,7 +7578,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>29907.365999999998</v>
       </c>
@@ -7704,40 +7704,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -9098,7 +9098,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>120876.05300000001</v>
       </c>
@@ -9142,10 +9142,10 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="11" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="11" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P38" sqref="P38"/>
+      <selection pane="bottomRight" activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9163,14 +9163,15 @@
     <col min="11" max="11" width="5" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
@@ -9178,7 +9179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>78</v>
       </c>
@@ -9186,8 +9187,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -9195,7 +9196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -9203,7 +9204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -9211,7 +9212,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -9219,49 +9220,49 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>81</v>
       </c>
@@ -9302,7 +9303,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
@@ -9343,7 +9344,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -9384,7 +9385,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -9425,7 +9426,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -9466,7 +9467,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>41</v>
       </c>
@@ -9507,7 +9508,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>42</v>
       </c>
@@ -9548,7 +9549,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>43</v>
       </c>
@@ -9589,7 +9590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
@@ -9630,7 +9631,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
@@ -9712,7 +9713,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
@@ -9753,7 +9754,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>48</v>
       </c>
@@ -9794,7 +9795,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
@@ -9835,7 +9836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>50</v>
       </c>
@@ -9876,7 +9877,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
@@ -9917,7 +9918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -9958,7 +9959,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
@@ -9999,7 +10000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
@@ -10040,7 +10041,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>55</v>
       </c>
@@ -10081,7 +10082,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>56</v>
       </c>
@@ -10122,7 +10123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>57</v>
       </c>
@@ -10163,7 +10164,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>58</v>
       </c>
@@ -10204,7 +10205,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>59</v>
       </c>
@@ -10245,7 +10246,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>60</v>
       </c>
@@ -10286,7 +10287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>61</v>
       </c>
@@ -10327,7 +10328,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>62</v>
       </c>
@@ -10368,7 +10369,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>63</v>
       </c>
@@ -10409,7 +10410,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>64</v>
       </c>
@@ -10450,7 +10451,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>65</v>
       </c>
@@ -10491,7 +10492,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>66</v>
       </c>
@@ -10532,7 +10533,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>67</v>
       </c>
@@ -10573,7 +10574,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>68</v>
       </c>
@@ -10618,7 +10619,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>491618.97399999993</v>
       </c>
@@ -10634,20 +10635,28 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <f>L45/3.6</f>
+        <v>136560.82611111109</v>
+      </c>
+      <c r="P46">
+        <f>M45/3.6</f>
+        <v>132439.50249999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>83</v>
       </c>
@@ -10655,7 +10664,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>89</v>
       </c>
@@ -10763,40 +10772,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -12157,7 +12166,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>246583.53699999998</v>
       </c>
@@ -12291,40 +12300,40 @@
       <c r="A10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" s="22" t="s">
+      <c r="G10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="24" t="s">
         <v>80</v>
       </c>
     </row>
@@ -13685,7 +13694,7 @@
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L45" s="23">
+      <c r="L45" s="20">
         <f>SUM(L13:L43)</f>
         <v>178258.52799999996</v>
       </c>

</xml_diff>